<commit_message>
Add Aulas iniciais LIMA HARE e SOP
</commit_message>
<xml_diff>
--- a/1des/Pre-turma-A.xlsx
+++ b/1des/Pre-turma-A.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Danilo Berimni Soares</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Felipe Henrique Lopes Gabriel</t>
+  </si>
+  <si>
+    <t>Augusto Cezar da Silva</t>
   </si>
 </sst>
 </file>
@@ -398,9 +401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -502,6 +507,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Aula 1 - SO
</commit_message>
<xml_diff>
--- a/1des/Pre-turma-A.xlsx
+++ b/1des/Pre-turma-A.xlsx
@@ -403,9 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -414,105 +412,108 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:A20">
+    <sortCondition ref="A20"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>